<commit_message>
Revisões de diagrama e Estrutura do Relatorio
1h
</commit_message>
<xml_diff>
--- a/Engenharia de Software/Tabela de atores e respetivos casos de uso.xlsx
+++ b/Engenharia de Software/Tabela de atores e respetivos casos de uso.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>Professor</t>
   </si>
@@ -41,63 +41,12 @@
     <t>Eliminar Inquérito</t>
   </si>
   <si>
-    <t>Responder questionario</t>
-  </si>
-  <si>
-    <t>Eliminar questionario</t>
-  </si>
-  <si>
-    <t>Consultar questionario</t>
-  </si>
-  <si>
-    <t>Criar utente</t>
-  </si>
-  <si>
-    <t>Consultar utente</t>
-  </si>
-  <si>
-    <t>Alterar utente</t>
-  </si>
-  <si>
-    <t>Eliminar utente</t>
-  </si>
-  <si>
-    <t>Alterar questionario</t>
-  </si>
-  <si>
-    <t>Comparar Trilho</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
-    <t>Consultar estabelecimentos para descansar</t>
-  </si>
-  <si>
-    <t>Visualizar condições metereologicas para o dia selecionado</t>
-  </si>
-  <si>
-    <t>selecionar o dia que deseja fazer o trilho</t>
-  </si>
-  <si>
     <t>Alterar dia que deseja fazer trilho</t>
   </si>
   <si>
-    <t>Selecionar guia</t>
-  </si>
-  <si>
-    <t>Alterar guia</t>
-  </si>
-  <si>
-    <t>Escolher guia</t>
-  </si>
-  <si>
-    <t>Mostrar contactos</t>
-  </si>
-  <si>
-    <t>Consultar testes trilho</t>
-  </si>
-  <si>
     <t>O que faz?</t>
   </si>
   <si>
@@ -135,6 +84,51 @@
   </si>
   <si>
     <t>Turista/Professor</t>
+  </si>
+  <si>
+    <t>Criar Turista</t>
+  </si>
+  <si>
+    <t>Consultar Turista</t>
+  </si>
+  <si>
+    <t>Alterar Turista</t>
+  </si>
+  <si>
+    <t>Eliminar Turista</t>
+  </si>
+  <si>
+    <t>Responder Questionario</t>
+  </si>
+  <si>
+    <t>Consultar Questionario</t>
+  </si>
+  <si>
+    <t>Visualizar Trilho Recomendado</t>
+  </si>
+  <si>
+    <t>Consultar Estabelecimentos para Descansar</t>
+  </si>
+  <si>
+    <t>Visualizar Condições Metereologicas para o dia selecionado</t>
+  </si>
+  <si>
+    <t>Selecionar o dia que deseja fazer o trilho</t>
+  </si>
+  <si>
+    <t>Selecionar Guia</t>
+  </si>
+  <si>
+    <t>Alterar Guia</t>
+  </si>
+  <si>
+    <t>Escolher Guia</t>
+  </si>
+  <si>
+    <t>Consultar Testes Trilho</t>
+  </si>
+  <si>
+    <t>Mostrar Contactos</t>
   </si>
 </sst>
 </file>
@@ -633,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,10 +650,10 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -711,10 +705,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -722,10 +716,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -733,21 +727,20 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -755,20 +748,21 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -776,10 +770,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -787,10 +781,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -798,10 +792,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -809,10 +803,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -820,10 +814,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -831,10 +825,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -842,7 +836,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>17</v>
@@ -850,13 +844,14 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -864,22 +859,21 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -887,10 +881,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -898,10 +892,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -909,10 +903,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -920,10 +914,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -934,7 +928,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -945,7 +939,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -956,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -967,46 +961,32 @@
         <v>0</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>31</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="A33" s="4"/>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="1"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
@@ -1018,15 +998,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+      <c r="B37" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>